<commit_message>
Chnged integrationPlan in Excel
</commit_message>
<xml_diff>
--- a/IntegrationPlan.xlsx
+++ b/IntegrationPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefanie Nielson\Documents\GitHub\MicrowaveHandIn2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3175B2CF-8977-4A7D-BE2A-4F0555A76CC0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D917DEEC-1CDB-4031-9511-CBD59251C025}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" xr2:uid="{14518D7A-741C-483D-AF6D-D7CEDCE24808}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
   <si>
     <t>Step</t>
   </si>
@@ -442,7 +442,7 @@
   <dimension ref="F5:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -541,7 +541,9 @@
       <c r="F9" s="3">
         <v>4</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H9" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>